<commit_message>
remove September data for testing
</commit_message>
<xml_diff>
--- a/excel_exports/石滩区分区计量.xlsx
+++ b/excel_exports/石滩区分区计量.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="107">
   <si>
     <t>石滩分区计量统计</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>合计:</t>
-  </si>
-  <si>
-    <t>2025年9月</t>
   </si>
   <si>
     <t>石滩区所有表册</t>
@@ -1749,10 +1746,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T66"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3279,199 +3276,8 @@
         <v>0.181604918232027</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="75" t="s">
-        <v>28</v>
-      </c>
-      <c r="B60" s="77"/>
-      <c r="C60" s="77"/>
-      <c r="D60" s="77"/>
-      <c r="E60" s="77"/>
-      <c r="F60" s="77"/>
-      <c r="G60" s="77"/>
-      <c r="H60" s="77"/>
-      <c r="I60" s="77"/>
-      <c r="J60" s="77"/>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="77"/>
-      <c r="B61" s="75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" s="77"/>
-      <c r="D61" s="77"/>
-      <c r="E61" s="77"/>
-      <c r="F61" s="77"/>
-      <c r="G61" s="75" t="s">
-        <v>9</v>
-      </c>
-      <c r="H61" s="77"/>
-      <c r="I61" s="77"/>
-      <c r="J61" s="77"/>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="75"/>
-      <c r="B62" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" s="75" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="G62" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="H62" s="75" t="s">
-        <v>16</v>
-      </c>
-      <c r="I62" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="J62" s="75" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="75" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" s="75">
-        <v>4264205</v>
-      </c>
-      <c r="C63" s="75">
-        <v>3457264</v>
-      </c>
-      <c r="D63" s="75">
-        <v>253250</v>
-      </c>
-      <c r="E63" s="75">
-        <v>0</v>
-      </c>
-      <c r="F63" s="75">
-        <v>0</v>
-      </c>
-      <c r="G63" s="75">
-        <f>B63-C63-D63</f>
-        <v>553691</v>
-      </c>
-      <c r="H63" s="75">
-        <v>223896</v>
-      </c>
-      <c r="I63" s="75">
-        <f>G63-H63</f>
-        <v>329795</v>
-      </c>
-      <c r="J63" s="79">
-        <f>I63/G63</f>
-        <v>0.595630053585845</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="75" t="s">
-        <v>25</v>
-      </c>
-      <c r="B64" s="75">
-        <v>0</v>
-      </c>
-      <c r="C64" s="75">
-        <v>0</v>
-      </c>
-      <c r="D64" s="75">
-        <v>253250</v>
-      </c>
-      <c r="E64" s="75">
-        <v>505577</v>
-      </c>
-      <c r="F64" s="75">
-        <v>265859</v>
-      </c>
-      <c r="G64" s="75">
-        <f>D64+E64-F64</f>
-        <v>492968</v>
-      </c>
-      <c r="H64" s="75">
-        <v>550454</v>
-      </c>
-      <c r="I64" s="75">
-        <f>G64-H64</f>
-        <v>-57486</v>
-      </c>
-      <c r="J64" s="79">
-        <f>I64/G64</f>
-        <v>-0.1166120316126</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="B65" s="75">
-        <v>0</v>
-      </c>
-      <c r="C65" s="75">
-        <v>0</v>
-      </c>
-      <c r="D65" s="75">
-        <v>0</v>
-      </c>
-      <c r="E65" s="75">
-        <v>0</v>
-      </c>
-      <c r="F65" s="75">
-        <v>265859</v>
-      </c>
-      <c r="G65" s="75">
-        <f>F65</f>
-        <v>265859</v>
-      </c>
-      <c r="H65" s="75">
-        <v>256399</v>
-      </c>
-      <c r="I65" s="75">
-        <f>G65-H65</f>
-        <v>9460</v>
-      </c>
-      <c r="J65" s="79">
-        <f>I65/G65</f>
-        <v>0.0355827713186313</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" s="75"/>
-      <c r="B66" s="75"/>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="G66" s="75">
-        <f>SUM(G63:G65)</f>
-        <v>1312518</v>
-      </c>
-      <c r="H66" s="75">
-        <f>SUM(H63:H65)</f>
-        <v>1030749</v>
-      </c>
-      <c r="I66" s="75">
-        <f>G66-H66</f>
-        <v>281769</v>
-      </c>
-      <c r="J66" s="79">
-        <f>I66/G66</f>
-        <v>0.214678198698989</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="29">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="A9:J9"/>
@@ -3501,9 +3307,6 @@
     <mergeCell ref="A52:J52"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="G53:J53"/>
-    <mergeCell ref="A60:J60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="G61:J61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3546,7 +3349,7 @@
     </row>
     <row r="2" spans="2:20">
       <c r="B2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="13"/>
@@ -3570,7 +3373,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="13"/>
@@ -3585,10 +3388,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="13"/>
@@ -3684,7 +3487,7 @@
     </row>
     <row r="10" spans="2:20">
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="8">
         <f>SUM(C8:C9)</f>
@@ -3747,13 +3550,13 @@
     </row>
     <row r="14" spans="2:20">
       <c r="B14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>15</v>
@@ -3831,7 +3634,7 @@
     </row>
     <row r="19" ht="25.5" customHeight="1" spans="2:8">
       <c r="B19" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -3842,7 +3645,7 @@
     </row>
     <row r="20" ht="26.25" customHeight="1" spans="2:8">
       <c r="B20" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -3853,7 +3656,7 @@
     </row>
     <row r="21" ht="27" customHeight="1" spans="2:2">
       <c r="B21" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="5:8">
@@ -3959,7 +3762,7 @@
     </row>
     <row r="2" spans="2:20">
       <c r="B2" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="13"/>
@@ -3983,7 +3786,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="13"/>
@@ -3998,10 +3801,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="13"/>
@@ -4097,7 +3900,7 @@
     </row>
     <row r="10" spans="2:20">
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="8">
         <f>SUM(C8:C9)</f>
@@ -4160,13 +3963,13 @@
     </row>
     <row r="14" spans="2:20">
       <c r="B14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>15</v>
@@ -4244,7 +4047,7 @@
     </row>
     <row r="19" ht="25.5" customHeight="1" spans="2:8">
       <c r="B19" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4255,7 +4058,7 @@
     </row>
     <row r="20" ht="26.25" customHeight="1" spans="2:8">
       <c r="B20" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -4266,7 +4069,7 @@
     </row>
     <row r="21" ht="27" customHeight="1" spans="2:2">
       <c r="B21" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="5:8">
@@ -4372,7 +4175,7 @@
     </row>
     <row r="2" spans="2:20">
       <c r="B2" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="13"/>
@@ -4396,7 +4199,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="13"/>
@@ -4411,10 +4214,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="13"/>
@@ -4510,7 +4313,7 @@
     </row>
     <row r="10" spans="2:20">
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="8">
         <f>SUM(C8:C9)</f>
@@ -4573,13 +4376,13 @@
     </row>
     <row r="14" spans="2:20">
       <c r="B14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>15</v>
@@ -4667,7 +4470,7 @@
     </row>
     <row r="19" ht="25.5" customHeight="1" spans="2:8">
       <c r="B19" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -4678,7 +4481,7 @@
     </row>
     <row r="20" ht="26.25" customHeight="1" spans="2:8">
       <c r="B20" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -4689,7 +4492,7 @@
     </row>
     <row r="21" ht="27" customHeight="1" spans="2:2">
       <c r="B21" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="5:8">
@@ -4795,7 +4598,7 @@
     </row>
     <row r="2" spans="2:20">
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="13"/>
@@ -4819,7 +4622,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="13"/>
@@ -4834,7 +4637,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="13"/>
@@ -4930,7 +4733,7 @@
     </row>
     <row r="11" spans="2:20">
       <c r="B11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="8">
         <f>SUM(C8:C10)</f>
@@ -4990,13 +4793,13 @@
     </row>
     <row r="15" spans="2:20">
       <c r="B15" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>15</v>
@@ -5079,7 +4882,7 @@
     </row>
     <row r="20" ht="25.5" customHeight="1" spans="2:8">
       <c r="B20" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -5090,7 +4893,7 @@
     </row>
     <row r="21" ht="26.25" customHeight="1" spans="2:8">
       <c r="B21" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -5101,7 +4904,7 @@
     </row>
     <row r="22" ht="27" customHeight="1" spans="2:2">
       <c r="B22" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="5:8">
@@ -5299,36 +5102,36 @@
   <sheetData>
     <row r="1" ht="28" customHeight="1" spans="1:1">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" ht="13.5" customHeight="1" spans="1:9">
       <c r="A2" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="C2" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="D2" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="E2" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="F2" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="G2" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="H2" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="I2" s="61" t="s">
         <v>37</v>
-      </c>
-      <c r="I2" s="61" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" spans="1:9">
@@ -5339,7 +5142,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="56">
         <v>29</v>
@@ -5357,7 +5160,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="62" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" spans="1:9">
@@ -5368,7 +5171,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="56">
         <v>889</v>
@@ -5386,7 +5189,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" spans="1:9">
@@ -5397,7 +5200,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="56">
         <v>1122</v>
@@ -5415,7 +5218,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" spans="1:9">
@@ -5426,7 +5229,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="56">
         <v>100</v>
@@ -5444,7 +5247,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" spans="1:9">
@@ -5452,7 +5255,7 @@
       <c r="B7" s="41"/>
       <c r="C7" s="63"/>
       <c r="D7" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="42">
         <f>SUM(E3:E6)</f>
@@ -5471,7 +5274,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="56">
         <v>126</v>
@@ -5489,7 +5292,7 @@
         <v>-4436</v>
       </c>
       <c r="I8" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" spans="1:9">
@@ -5500,7 +5303,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="56">
         <v>118</v>
@@ -5518,7 +5321,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" spans="1:9">
@@ -5529,7 +5332,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="66">
         <v>1637</v>
@@ -5547,7 +5350,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" spans="1:9">
@@ -5558,7 +5361,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="56">
         <v>1358</v>
@@ -5576,7 +5379,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="62" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" spans="1:9">
@@ -5587,7 +5390,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="56">
         <v>1534</v>
@@ -5605,7 +5408,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" spans="1:9">
@@ -5616,7 +5419,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="56">
         <v>1154</v>
@@ -5634,7 +5437,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="62" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" spans="1:9">
@@ -5645,7 +5448,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="56">
         <v>133</v>
@@ -5663,7 +5466,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" spans="1:9">
@@ -5674,7 +5477,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="56">
         <v>638</v>
@@ -5692,7 +5495,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1" spans="1:9">
@@ -5703,7 +5506,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="56">
         <v>608</v>
@@ -5721,7 +5524,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="62" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1" spans="1:9">
@@ -5732,7 +5535,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="56">
         <v>855</v>
@@ -5750,7 +5553,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1" spans="1:9">
@@ -5761,7 +5564,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="56">
         <v>1128</v>
@@ -5779,7 +5582,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1" spans="1:9">
@@ -5790,7 +5593,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="56">
         <v>947</v>
@@ -5808,7 +5611,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1" spans="1:9">
@@ -5819,7 +5622,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="56">
         <v>520</v>
@@ -5837,7 +5640,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1" spans="1:9">
@@ -5848,7 +5651,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="56">
         <v>98</v>
@@ -5866,7 +5669,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1" spans="1:9">
@@ -5877,7 +5680,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="56">
         <v>75</v>
@@ -5895,7 +5698,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1" spans="1:9">
@@ -5906,7 +5709,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="66">
         <v>143</v>
@@ -5924,7 +5727,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1" spans="1:9">
@@ -5935,7 +5738,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="56">
         <v>140</v>
@@ -5953,7 +5756,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1" spans="1:9">
@@ -5964,7 +5767,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="56">
         <v>169</v>
@@ -5982,7 +5785,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1" spans="1:9">
@@ -5993,7 +5796,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="56">
         <v>397</v>
@@ -6011,7 +5814,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1" spans="1:9">
@@ -6022,7 +5825,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="56">
         <v>104</v>
@@ -6040,7 +5843,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1" spans="1:9">
@@ -6051,7 +5854,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="56">
         <v>104</v>
@@ -6069,7 +5872,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1" spans="1:9">
@@ -6080,7 +5883,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="56">
         <v>52</v>
@@ -6098,7 +5901,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1" spans="1:9">
@@ -6109,7 +5912,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="56">
         <v>188</v>
@@ -6127,7 +5930,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1" spans="1:9">
@@ -6138,7 +5941,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D31" s="56">
         <v>188</v>
@@ -6156,7 +5959,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1" spans="1:9">
@@ -6167,7 +5970,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="56">
         <v>110</v>
@@ -6185,7 +5988,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1" spans="1:9">
@@ -6196,7 +5999,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="56">
         <v>226</v>
@@ -6214,7 +6017,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1" spans="1:9">
@@ -6225,7 +6028,7 @@
         <v>3</v>
       </c>
       <c r="C34" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34" s="56">
         <v>192</v>
@@ -6243,7 +6046,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" ht="13.5" customHeight="1" spans="1:9">
@@ -6254,7 +6057,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35" s="56">
         <v>176</v>
@@ -6272,7 +6075,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" ht="13.5" customHeight="1" spans="1:9">
@@ -6283,7 +6086,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="56">
         <v>176</v>
@@ -6301,7 +6104,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" ht="13.5" customHeight="1" spans="1:9">
@@ -6312,7 +6115,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" s="56">
         <v>104</v>
@@ -6330,7 +6133,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" ht="13.5" customHeight="1" spans="1:9">
@@ -6341,7 +6144,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38" s="56">
         <v>76</v>
@@ -6359,7 +6162,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" ht="13.5" customHeight="1" spans="1:9">
@@ -6370,7 +6173,7 @@
         <v>3</v>
       </c>
       <c r="C39" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39" s="56">
         <v>1215</v>
@@ -6388,7 +6191,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" ht="13.5" customHeight="1" spans="1:9">
@@ -6399,7 +6202,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" s="56">
         <v>517</v>
@@ -6417,7 +6220,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" ht="13.5" customHeight="1" spans="1:9">
@@ -6428,7 +6231,7 @@
         <v>3</v>
       </c>
       <c r="C41" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" s="56">
         <v>189</v>
@@ -6446,7 +6249,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" ht="13.5" customHeight="1" spans="1:9">
@@ -6457,7 +6260,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D42" s="66">
         <v>189</v>
@@ -6475,7 +6278,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" ht="13.5" customHeight="1" spans="1:9">
@@ -6486,7 +6289,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D43" s="56">
         <v>189</v>
@@ -6504,7 +6307,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" ht="13.5" customHeight="1" spans="1:9">
@@ -6515,7 +6318,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D44" s="56">
         <v>109</v>
@@ -6533,7 +6336,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" ht="13.5" customHeight="1" spans="1:9">
@@ -6544,7 +6347,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D45" s="56">
         <v>11</v>
@@ -6562,7 +6365,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" ht="13.5" customHeight="1" spans="1:9">
@@ -6573,7 +6376,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D46" s="56">
         <v>352</v>
@@ -6591,7 +6394,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" ht="13.5" customHeight="1" spans="1:9">
@@ -6602,7 +6405,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D47" s="56">
         <v>41</v>
@@ -6620,7 +6423,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" ht="13.5" customHeight="1" spans="1:9">
@@ -6631,7 +6434,7 @@
         <v>2</v>
       </c>
       <c r="C48" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D48" s="56">
         <v>124</v>
@@ -6649,7 +6452,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" ht="13.5" customHeight="1" spans="1:9">
@@ -6660,7 +6463,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D49" s="56">
         <v>168</v>
@@ -6678,7 +6481,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" ht="13.5" customHeight="1" spans="1:9">
@@ -6689,7 +6492,7 @@
         <v>2</v>
       </c>
       <c r="C50" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D50" s="56">
         <v>192</v>
@@ -6707,7 +6510,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" ht="13.5" customHeight="1" spans="1:9">
@@ -6718,7 +6521,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D51" s="56">
         <v>76</v>
@@ -6736,7 +6539,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" ht="13.5" customHeight="1" spans="1:9">
@@ -6747,7 +6550,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D52" s="56">
         <v>77</v>
@@ -6765,7 +6568,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" ht="13.5" customHeight="1" spans="1:9">
@@ -6776,7 +6579,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D53" s="56">
         <v>78</v>
@@ -6794,7 +6597,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" ht="13.5" customHeight="1" spans="1:9">
@@ -6805,7 +6608,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D54" s="56">
         <v>175</v>
@@ -6823,7 +6626,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" ht="13.5" customHeight="1" spans="1:9">
@@ -6834,7 +6637,7 @@
         <v>2</v>
       </c>
       <c r="C55" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D55" s="56">
         <v>176</v>
@@ -6852,7 +6655,7 @@
         <v>0</v>
       </c>
       <c r="I55" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" ht="13.5" customHeight="1" spans="1:9">
@@ -6863,7 +6666,7 @@
         <v>2</v>
       </c>
       <c r="C56" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D56" s="56">
         <v>176</v>
@@ -6881,7 +6684,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" ht="13.5" customHeight="1" spans="1:9">
@@ -6892,7 +6695,7 @@
         <v>2</v>
       </c>
       <c r="C57" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D57" s="56">
         <v>88</v>
@@ -6910,7 +6713,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" ht="13.5" customHeight="1" spans="1:9">
@@ -6921,7 +6724,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D58" s="56">
         <v>220</v>
@@ -6939,7 +6742,7 @@
         <v>0</v>
       </c>
       <c r="I58" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1" spans="1:9">
@@ -6950,7 +6753,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D59" s="56">
         <v>157</v>
@@ -6968,7 +6771,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" ht="13.5" customHeight="1" spans="1:9">
@@ -6979,7 +6782,7 @@
         <v>2</v>
       </c>
       <c r="C60" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D60" s="56">
         <v>224</v>
@@ -6997,7 +6800,7 @@
         <v>0</v>
       </c>
       <c r="I60" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" ht="13.5" customHeight="1" spans="1:9">
@@ -7008,7 +6811,7 @@
         <v>2</v>
       </c>
       <c r="C61" s="60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D61" s="66">
         <v>226</v>
@@ -7026,7 +6829,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" ht="13.5" customHeight="1" spans="1:9">
@@ -7037,7 +6840,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D62" s="56">
         <v>233</v>
@@ -7055,7 +6858,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" ht="13.5" customHeight="1" spans="1:9">
@@ -7066,7 +6869,7 @@
         <v>2</v>
       </c>
       <c r="C63" s="67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D63" s="56">
         <v>240</v>
@@ -7084,7 +6887,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" ht="13.5" customHeight="1" spans="1:9">
@@ -7095,7 +6898,7 @@
         <v>2</v>
       </c>
       <c r="C64" s="67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D64" s="56">
         <v>212</v>
@@ -7113,7 +6916,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" ht="13.5" customHeight="1" spans="1:9">
@@ -7124,7 +6927,7 @@
         <v>2</v>
       </c>
       <c r="C65" s="67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D65" s="56">
         <v>176</v>
@@ -7142,7 +6945,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="68" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" ht="13.5" customHeight="1" spans="1:9">
@@ -7153,7 +6956,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D66" s="56">
         <v>2666</v>
@@ -7171,7 +6974,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" ht="13.5" customHeight="1" spans="1:9">
@@ -7182,7 +6985,7 @@
         <v>2</v>
       </c>
       <c r="C67" s="67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D67" s="56">
         <v>1168</v>
@@ -7200,7 +7003,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" ht="13.5" customHeight="1" spans="1:9">
@@ -7208,7 +7011,7 @@
       <c r="B68" s="41"/>
       <c r="C68" s="69"/>
       <c r="D68" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E68" s="42">
         <f>SUM(E8:E67)</f>
@@ -7227,7 +7030,7 @@
         <v>3</v>
       </c>
       <c r="C69" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D69" s="56">
         <v>180</v>
@@ -7245,7 +7048,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" ht="13.5" customHeight="1" spans="1:9">
@@ -7256,7 +7059,7 @@
         <v>3</v>
       </c>
       <c r="C70" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D70" s="56">
         <v>219</v>
@@ -7274,7 +7077,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" ht="13.5" customHeight="1" spans="1:9">
@@ -7285,7 +7088,7 @@
         <v>3</v>
       </c>
       <c r="C71" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D71" s="56">
         <v>245</v>
@@ -7303,7 +7106,7 @@
         <v>0</v>
       </c>
       <c r="I71" s="62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" ht="13.5" customHeight="1" spans="1:9">
@@ -7314,7 +7117,7 @@
         <v>3</v>
       </c>
       <c r="C72" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D72" s="56">
         <v>120</v>
@@ -7332,7 +7135,7 @@
         <v>0</v>
       </c>
       <c r="I72" s="62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" ht="13.5" customHeight="1" spans="1:9">
@@ -7343,7 +7146,7 @@
         <v>3</v>
       </c>
       <c r="C73" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D73" s="56">
         <v>35</v>
@@ -7361,7 +7164,7 @@
         <v>0</v>
       </c>
       <c r="I73" s="62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" ht="13.5" customHeight="1" spans="1:9">
@@ -7372,7 +7175,7 @@
         <v>3</v>
       </c>
       <c r="C74" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D74" s="56">
         <v>200</v>
@@ -7390,7 +7193,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" ht="13.5" customHeight="1" spans="1:9">
@@ -7401,7 +7204,7 @@
         <v>3</v>
       </c>
       <c r="C75" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D75" s="56">
         <v>305</v>
@@ -7419,7 +7222,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="76" ht="13.5" customHeight="1" spans="1:9">
@@ -7430,7 +7233,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D76" s="56">
         <v>98</v>
@@ -7448,7 +7251,7 @@
         <v>0</v>
       </c>
       <c r="I76" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="77" ht="13.5" customHeight="1" spans="1:9">
@@ -7459,7 +7262,7 @@
         <v>3</v>
       </c>
       <c r="C77" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D77" s="56">
         <v>156</v>
@@ -7477,7 +7280,7 @@
         <v>0</v>
       </c>
       <c r="I77" s="62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" ht="13.5" customHeight="1" spans="1:9">
@@ -7488,7 +7291,7 @@
         <v>3</v>
       </c>
       <c r="C78" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D78" s="56">
         <v>119</v>
@@ -7506,7 +7309,7 @@
         <v>0</v>
       </c>
       <c r="I78" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="79" ht="13.5" customHeight="1" spans="1:9">
@@ -7517,7 +7320,7 @@
         <v>3</v>
       </c>
       <c r="C79" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D79" s="56">
         <v>259</v>
@@ -7535,7 +7338,7 @@
         <v>0</v>
       </c>
       <c r="I79" s="62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="80" ht="13.5" customHeight="1" spans="1:9">
@@ -7546,7 +7349,7 @@
         <v>3</v>
       </c>
       <c r="C80" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D80" s="56">
         <v>201</v>
@@ -7564,7 +7367,7 @@
         <v>0</v>
       </c>
       <c r="I80" s="62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="81" ht="13.5" customHeight="1" spans="1:9">
@@ -7575,7 +7378,7 @@
         <v>3</v>
       </c>
       <c r="C81" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D81" s="56">
         <v>234</v>
@@ -7593,7 +7396,7 @@
         <v>0</v>
       </c>
       <c r="I81" s="62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" ht="13.5" customHeight="1" spans="1:9">
@@ -7604,7 +7407,7 @@
         <v>3</v>
       </c>
       <c r="C82" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D82" s="56">
         <v>203</v>
@@ -7622,7 +7425,7 @@
         <v>0</v>
       </c>
       <c r="I82" s="62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" ht="13.5" customHeight="1" spans="1:9">
@@ -7633,7 +7436,7 @@
         <v>3</v>
       </c>
       <c r="C83" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D83" s="56">
         <v>97</v>
@@ -7651,7 +7454,7 @@
         <v>0</v>
       </c>
       <c r="I83" s="62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84" ht="13.5" customHeight="1" spans="1:9">
@@ -7662,7 +7465,7 @@
         <v>3</v>
       </c>
       <c r="C84" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D84" s="56">
         <v>191</v>
@@ -7680,7 +7483,7 @@
         <v>0</v>
       </c>
       <c r="I84" s="62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" ht="13.5" customHeight="1" spans="1:9">
@@ -7691,7 +7494,7 @@
         <v>3</v>
       </c>
       <c r="C85" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D85" s="56">
         <v>164</v>
@@ -7709,7 +7512,7 @@
         <v>0</v>
       </c>
       <c r="I85" s="62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" ht="11.25" customHeight="1" spans="1:9">
@@ -7720,7 +7523,7 @@
         <v>3</v>
       </c>
       <c r="C86" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D86" s="56">
         <v>167</v>
@@ -7738,7 +7541,7 @@
         <v>0</v>
       </c>
       <c r="I86" s="62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" ht="13.5" customHeight="1" spans="1:9">
@@ -7749,7 +7552,7 @@
         <v>3</v>
       </c>
       <c r="C87" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D87" s="56">
         <v>72</v>
@@ -7767,7 +7570,7 @@
         <v>0</v>
       </c>
       <c r="I87" s="62" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" ht="13.5" customHeight="1" spans="1:9">
@@ -7778,7 +7581,7 @@
         <v>3</v>
       </c>
       <c r="C88" s="60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D88" s="66">
         <v>204</v>
@@ -7796,7 +7599,7 @@
         <v>0</v>
       </c>
       <c r="I88" s="60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="89" ht="13.5" customHeight="1" spans="1:9">
@@ -7807,7 +7610,7 @@
         <v>3</v>
       </c>
       <c r="C89" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D89" s="56">
         <v>146</v>
@@ -7825,7 +7628,7 @@
         <v>0</v>
       </c>
       <c r="I89" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="90" ht="13.5" customHeight="1" spans="1:9">
@@ -7836,7 +7639,7 @@
         <v>3</v>
       </c>
       <c r="C90" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D90" s="56">
         <v>87</v>
@@ -7854,7 +7657,7 @@
         <v>0</v>
       </c>
       <c r="I90" s="62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="91" ht="13.5" customHeight="1" spans="1:9">
@@ -7865,7 +7668,7 @@
         <v>3</v>
       </c>
       <c r="C91" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D91" s="56">
         <v>224</v>
@@ -7883,7 +7686,7 @@
         <v>0</v>
       </c>
       <c r="I91" s="62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="92" ht="13.5" customHeight="1" spans="1:9">
@@ -7894,7 +7697,7 @@
         <v>3</v>
       </c>
       <c r="C92" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D92" s="56">
         <v>50</v>
@@ -7912,7 +7715,7 @@
         <v>0</v>
       </c>
       <c r="I92" s="62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="93" ht="13.5" customHeight="1" spans="1:9">
@@ -7923,7 +7726,7 @@
         <v>3</v>
       </c>
       <c r="C93" s="67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D93" s="56">
         <v>386</v>
@@ -7941,7 +7744,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -7949,7 +7752,7 @@
       <c r="B94" s="43"/>
       <c r="C94" s="70"/>
       <c r="D94" s="71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E94" s="53">
         <f>SUM(E69:E93)</f>
@@ -7968,7 +7771,7 @@
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -7976,19 +7779,19 @@
         <v>1</v>
       </c>
       <c r="B99" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="D99" s="6"/>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B100" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="102" spans="3:6">
@@ -8064,7 +7867,7 @@
     </row>
     <row r="106" spans="2:6">
       <c r="B106" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C106">
         <f>SUM(C103:C105)</f>
@@ -8210,7 +8013,7 @@
   <sheetData>
     <row r="1" ht="28" customHeight="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -8218,19 +8021,19 @@
     </row>
     <row r="2" ht="13.5" customHeight="1" spans="1:8">
       <c r="A2" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="28" t="s">
+      <c r="E2" s="28" t="s">
         <v>70</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>71</v>
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="30"/>
@@ -10054,7 +9857,7 @@
     </row>
     <row r="97" spans="2:2">
       <c r="B97" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99" spans="2:3">
@@ -10062,7 +9865,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="100" spans="2:3">
@@ -10070,7 +9873,7 @@
         <v>3</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="102" spans="3:6">
@@ -10146,7 +9949,7 @@
     </row>
     <row r="106" spans="2:6">
       <c r="B106" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C106">
         <f>SUM(C103:C105)</f>
@@ -10322,7 +10125,7 @@
   <sheetData>
     <row r="1" ht="28" customHeight="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -10330,16 +10133,16 @@
     </row>
     <row r="2" ht="13.5" customHeight="1" spans="1:8">
       <c r="A2" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>69</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>70</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
@@ -12265,7 +12068,7 @@
     </row>
     <row r="97" spans="2:20">
       <c r="B97" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M97" s="12"/>
       <c r="N97" s="13"/>
@@ -12287,7 +12090,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M99" s="12"/>
       <c r="N99" s="13"/>
@@ -12301,7 +12104,7 @@
         <v>3</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M100" s="12"/>
       <c r="N100" s="13"/>
@@ -12415,7 +12218,7 @@
     </row>
     <row r="106" spans="2:20">
       <c r="B106" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C106">
         <f>SUM(C103:C105)</f>
@@ -12625,7 +12428,7 @@
   <sheetData>
     <row r="1" ht="28" customHeight="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -12633,16 +12436,16 @@
     </row>
     <row r="2" ht="13.5" customHeight="1" spans="1:8">
       <c r="A2" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>69</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>70</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
@@ -14577,7 +14380,7 @@
     </row>
     <row r="97" spans="2:20">
       <c r="B97" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M97" s="12"/>
       <c r="N97" s="13"/>
@@ -14601,7 +14404,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M99" s="12"/>
       <c r="N99" s="13"/>
@@ -14616,7 +14419,7 @@
         <v>3</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M100" s="12"/>
       <c r="N100" s="13"/>
@@ -14736,7 +14539,7 @@
     </row>
     <row r="106" spans="2:20">
       <c r="B106" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C106">
         <f>SUM(C103:C105)</f>
@@ -14964,7 +14767,7 @@
     </row>
     <row r="2" spans="2:20">
       <c r="B2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="13"/>
@@ -14988,7 +14791,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="13"/>
@@ -15003,7 +14806,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="13"/>
@@ -15123,7 +14926,7 @@
     </row>
     <row r="11" spans="2:20">
       <c r="B11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="8">
         <f>SUM(C8:C10)</f>
@@ -15368,7 +15171,7 @@
     </row>
     <row r="2" spans="2:20">
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J2"/>
       <c r="M2" s="12"/>
@@ -15394,7 +15197,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J4"/>
       <c r="M4" s="12"/>
@@ -15410,7 +15213,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J5"/>
       <c r="M5" s="12"/>
@@ -15539,7 +15342,7 @@
     </row>
     <row r="11" spans="2:20">
       <c r="B11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="8">
         <f>SUM(C8:C10)</f>
@@ -15842,7 +15645,7 @@
     </row>
     <row r="2" spans="2:20">
       <c r="B2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J2"/>
       <c r="M2" s="12"/>
@@ -15868,7 +15671,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J4"/>
       <c r="M4" s="12"/>
@@ -15884,7 +15687,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J5"/>
       <c r="M5" s="12"/>
@@ -16013,7 +15816,7 @@
     </row>
     <row r="11" spans="2:20">
       <c r="B11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="8">
         <f>SUM(C8:C10)</f>
@@ -16339,7 +16142,7 @@
     </row>
     <row r="2" spans="2:20">
       <c r="B2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="13"/>
@@ -16363,7 +16166,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="13"/>
@@ -16378,7 +16181,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="13"/>
@@ -16501,7 +16304,7 @@
     </row>
     <row r="11" spans="2:20">
       <c r="B11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="8">
         <f>SUM(C8:C10)</f>

</xml_diff>

<commit_message>
Add partition meter view feature
</commit_message>
<xml_diff>
--- a/excel_exports/石滩区分区计量.xlsx
+++ b/excel_exports/石滩区分区计量.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="23">
   <si>
     <t>石滩分区计量统计</t>
   </si>
@@ -97,21 +97,6 @@
   <si>
     <t>合计：</t>
   </si>
-  <si>
-    <t>2025年5月</t>
-  </si>
-  <si>
-    <t>1 区</t>
-  </si>
-  <si>
-    <t>2 区</t>
-  </si>
-  <si>
-    <t>3 区</t>
-  </si>
-  <si>
-    <t>合计:</t>
-  </si>
 </sst>
 </file>
 
@@ -142,7 +127,7 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -491,7 +476,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -535,45 +520,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -701,7 +647,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
@@ -713,34 +659,34 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="11">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0">
@@ -825,7 +771,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -839,12 +785,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="57" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -865,22 +817,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1229,10 +1172,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A77" sqref="$A39:$XFD77"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K45" sqref="K$1:U$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1247,747 +1190,629 @@
     <col min="8" max="8" width="14.4247787610619" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.5309734513274" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.8761061946903" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.716814159292" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1592920353982" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="46" customHeight="1" spans="1:20">
+    <row r="1" ht="46" customHeight="1" spans="1:1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="20"/>
-      <c r="O1"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="20"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="20"/>
-    </row>
-    <row r="2" spans="10:20">
+    </row>
+    <row r="2" spans="10:10">
       <c r="J2"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="20"/>
-      <c r="O2"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="20"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="20"/>
-    </row>
-    <row r="3" spans="2:20">
+    </row>
+    <row r="3" spans="2:10">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="5"/>
       <c r="J3"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20"/>
-      <c r="O3"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="20"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="20"/>
-    </row>
-    <row r="4" spans="2:20">
+    </row>
+    <row r="4" spans="2:10">
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="5"/>
       <c r="J4"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="20"/>
-      <c r="O4"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="20"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="20"/>
-    </row>
-    <row r="5" ht="25.5" customHeight="1" spans="2:8">
-      <c r="B5" s="4" t="s">
+    </row>
+    <row r="5" ht="25.5" customHeight="1" spans="2:10">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" ht="26.25" customHeight="1" spans="2:8">
-      <c r="B6" s="4" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" ht="26.25" customHeight="1" spans="2:10">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" ht="27" customHeight="1" spans="2:2">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:20">
+    <row r="8" spans="2:10">
       <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="8"/>
       <c r="J8"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="20"/>
-      <c r="O8"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="20"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="20"/>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="7">
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="9">
         <v>45689</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="11"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="20"/>
-      <c r="O9"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="20"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="20"/>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="11"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="20"/>
-      <c r="O10"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="20"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="20"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="20"/>
-      <c r="O11"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="20"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="20"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="12" t="s">
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="12">
         <v>2611562</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="15">
         <v>2140549</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="15">
         <v>92714</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13">
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15">
         <f>B12-C12-D12</f>
         <v>378299</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="15">
         <v>175104</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="15">
         <f>G12-H12</f>
         <v>203195</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="19">
         <f>I12/G12</f>
         <v>0.537128038932167</v>
       </c>
-      <c r="O12"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="20"/>
-      <c r="S12"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="12" t="s">
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15">
         <v>92714</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="15">
         <v>574890</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="15">
         <v>280209</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="15">
         <f>D13+E13-F13</f>
         <v>387395</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="15">
         <v>456938</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="15">
         <f>G13-H13</f>
         <v>-69543</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="19">
         <f>I13/G13</f>
         <v>-0.179514449076524</v>
       </c>
-      <c r="O13"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="20"/>
-      <c r="S13"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15">
         <v>280209</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="15">
         <f>F14</f>
         <v>280209</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="15">
         <v>260128</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="15">
         <f>G14-H14</f>
         <v>20081</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="19">
         <f>I14/G14</f>
         <v>0.0716643648134071</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="13">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="15">
         <f>SUM(G12:G14)</f>
         <v>1045903</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="15">
         <f>SUM(H12:H14)</f>
         <v>892170</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="15">
         <f>G15-H15</f>
         <v>153733</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="19">
         <f>I15/G15</f>
         <v>0.146985905958774</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="7">
+    <row r="16" spans="1:10">
+      <c r="A16" s="9">
         <v>45717</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="11"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="20"/>
-      <c r="O16"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="20"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="20"/>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="10" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="11"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="20"/>
-      <c r="O17"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="20"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="20"/>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10" t="s">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M18" s="19"/>
-      <c r="N18" s="20"/>
-      <c r="O18"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="20"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="20"/>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="12" t="s">
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="12">
         <v>3888850</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="15">
         <v>3209501</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="15">
         <v>165239</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13">
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15">
         <f>B19-C19-D19</f>
         <v>514110</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="15">
         <v>200262</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="15">
         <f>G19-H19</f>
         <v>313848</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="19">
         <f>I19/G19</f>
         <v>0.610468576763728</v>
       </c>
-      <c r="O19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="20"/>
-      <c r="S19"/>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="12" t="s">
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15">
         <v>165239</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="15">
         <v>520457</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="15">
         <v>254750</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="15">
         <f>D20+E20-F20</f>
         <v>430946</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="15">
         <v>483259</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="15">
         <f>G20-H20</f>
         <v>-52313</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="19">
         <f>I20/G20</f>
         <v>-0.12139107916073</v>
       </c>
-      <c r="O20"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="20"/>
-      <c r="S20"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15">
         <v>254750</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="15">
         <f>F21</f>
         <v>254750</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="15">
         <v>219695</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="15">
         <f>G21-H21</f>
         <v>35055</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="19">
         <f>I21/G21</f>
         <v>0.137605495583906</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="13">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="15">
         <f>SUM(G19:G21)</f>
         <v>1199806</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="15">
         <f>SUM(H19:H21)</f>
         <v>903216</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="15">
         <f>G22-H22</f>
         <v>296590</v>
       </c>
-      <c r="J22" s="21">
+      <c r="J22" s="19">
         <f>I22/G22</f>
         <v>0.247198297058024</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="7">
+    <row r="23" spans="1:10">
+      <c r="A23" s="9">
         <v>45748</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="11"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="20"/>
-      <c r="O23"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="20"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="20"/>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10" t="s">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="10" t="s">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="11"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="20"/>
-      <c r="O24"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="20"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="20"/>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10" t="s">
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="M25" s="19"/>
-      <c r="N25" s="20"/>
-      <c r="O25"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="20"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="20"/>
-    </row>
-    <row r="26" spans="1:19">
-      <c r="A26" s="12" t="s">
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="15">
         <v>4535700</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="15">
         <v>3727121</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="15">
         <v>224316</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13">
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15">
         <f>B26-C26-D26</f>
         <v>584263</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="15">
         <v>231704</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="15">
         <f>G26-H26</f>
         <v>352559</v>
       </c>
-      <c r="J26" s="21">
+      <c r="J26" s="19">
         <f>I26/G26</f>
         <v>0.603425169829341</v>
       </c>
-      <c r="O26"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="20"/>
-      <c r="S26"/>
-    </row>
-    <row r="27" spans="1:19">
-      <c r="A27" s="12" t="s">
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15">
         <v>224316</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="15">
         <v>524848</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="15">
         <v>272594</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="15">
         <f>D27+E27-F27</f>
         <v>476570</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="15">
         <v>540112</v>
       </c>
-      <c r="I27" s="13">
+      <c r="I27" s="15">
         <f>G27-H27</f>
         <v>-63542</v>
       </c>
-      <c r="J27" s="21">
+      <c r="J27" s="19">
         <f>I27/G27</f>
         <v>-0.133331934448245</v>
       </c>
-      <c r="O27"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="20"/>
-      <c r="S27"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15">
         <v>272594</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="15">
         <f>F28</f>
         <v>272594</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="15">
         <v>250374</v>
       </c>
-      <c r="I28" s="13">
+      <c r="I28" s="15">
         <f>G28-H28</f>
         <v>22220</v>
       </c>
-      <c r="J28" s="21">
+      <c r="J28" s="19">
         <f>I28/G28</f>
         <v>0.0815131661005011</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="13">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="15">
         <f>SUM(G26:G28)</f>
         <v>1333427</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="15">
         <f>SUM(H26:H28)</f>
         <v>1022190</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="15">
         <f>G29-H29</f>
         <v>311237</v>
       </c>
-      <c r="J29" s="21">
+      <c r="J29" s="19">
         <f>I29/G29</f>
         <v>0.233411352852462</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="18"/>
+      <c r="A31" s="9">
+        <v>45778</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="13"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="17"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="18"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="13"/>
       <c r="G32" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="18"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="13"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="15"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="15" t="s">
         <v>10</v>
       </c>
@@ -2017,139 +1842,827 @@
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="15" t="s">
-        <v>24</v>
+      <c r="A34" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="B34" s="15">
-        <v>4149832</v>
+        <v>4299104</v>
       </c>
       <c r="C34" s="15">
-        <v>3378216</v>
+        <v>3499161</v>
       </c>
       <c r="D34" s="15">
-        <v>236130</v>
-      </c>
-      <c r="E34" s="15">
-        <v>0</v>
-      </c>
-      <c r="F34" s="15">
-        <v>0</v>
-      </c>
+        <v>244858</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
       <c r="G34" s="15">
         <f>B34-C34-D34</f>
-        <v>535486</v>
+        <v>555085</v>
       </c>
       <c r="H34" s="15">
-        <v>234672</v>
+        <v>230214</v>
       </c>
       <c r="I34" s="15">
-        <f>G34-H34</f>
-        <v>300814</v>
-      </c>
-      <c r="J34" s="22">
-        <f>I34/G34</f>
-        <v>0.561758850838304</v>
+        <f t="shared" ref="I34:I37" si="0">G34-H34</f>
+        <v>324871</v>
+      </c>
+      <c r="J34" s="19">
+        <f t="shared" ref="J34:J37" si="1">I34/G34</f>
+        <v>0.585263518199915</v>
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="15">
-        <v>0</v>
-      </c>
-      <c r="C35" s="15">
-        <v>0</v>
-      </c>
+      <c r="A35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="15">
-        <v>236130</v>
+        <v>244858</v>
       </c>
       <c r="E35" s="15">
-        <v>485583</v>
+        <v>501898</v>
       </c>
       <c r="F35" s="15">
-        <v>250686</v>
+        <v>258803</v>
       </c>
       <c r="G35" s="15">
         <f>D35+E35-F35</f>
-        <v>471027</v>
+        <v>487953</v>
       </c>
       <c r="H35" s="15">
-        <v>123689</v>
+        <v>545451</v>
       </c>
       <c r="I35" s="15">
-        <f>G35-H35</f>
-        <v>347338</v>
-      </c>
-      <c r="J35" s="22">
-        <f>I35/G35</f>
-        <v>0.73740571134988</v>
+        <f t="shared" si="0"/>
+        <v>-57498</v>
+      </c>
+      <c r="J35" s="19">
+        <f t="shared" si="1"/>
+        <v>-0.117835119366005</v>
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="15">
-        <v>0</v>
-      </c>
-      <c r="C36" s="15">
-        <v>0</v>
-      </c>
-      <c r="D36" s="15">
-        <v>0</v>
-      </c>
-      <c r="E36" s="15">
-        <v>0</v>
-      </c>
+      <c r="A36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
       <c r="F36" s="15">
-        <v>250686</v>
+        <v>258803</v>
       </c>
       <c r="G36" s="15">
         <f>F36</f>
-        <v>250686</v>
+        <v>258803</v>
       </c>
       <c r="H36" s="15">
-        <v>467568</v>
+        <v>246109</v>
       </c>
       <c r="I36" s="15">
-        <f>G36-H36</f>
-        <v>-216882</v>
-      </c>
-      <c r="J36" s="22">
-        <f>I36/G36</f>
-        <v>-0.865154017376319</v>
+        <f t="shared" si="0"/>
+        <v>12694</v>
+      </c>
+      <c r="J36" s="19">
+        <f t="shared" si="1"/>
+        <v>0.0490488904688122</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15" t="s">
-        <v>27</v>
-      </c>
+      <c r="A37" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="13"/>
       <c r="G37" s="15">
         <f>SUM(G34:G36)</f>
-        <v>1257199</v>
+        <v>1301841</v>
       </c>
       <c r="H37" s="15">
         <f>SUM(H34:H36)</f>
-        <v>825929</v>
+        <v>1021774</v>
       </c>
       <c r="I37" s="15">
-        <f>G37-H37</f>
-        <v>431270</v>
-      </c>
-      <c r="J37" s="22">
-        <f>I37/G37</f>
-        <v>0.343040361947472</v>
+        <f t="shared" si="0"/>
+        <v>280067</v>
+      </c>
+      <c r="J37" s="19">
+        <f t="shared" si="1"/>
+        <v>0.215131494552714</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="9">
+        <v>45809</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="11"/>
+      <c r="B39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="11"/>
+      <c r="B40" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="15">
+        <v>4312551</v>
+      </c>
+      <c r="C41" s="15">
+        <v>3504653</v>
+      </c>
+      <c r="D41" s="15">
+        <v>244504</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15">
+        <f>B41-C41-D41</f>
+        <v>563394</v>
+      </c>
+      <c r="H41" s="15">
+        <v>256745</v>
+      </c>
+      <c r="I41" s="15">
+        <f t="shared" ref="I36:I44" si="2">G41-H41</f>
+        <v>306649</v>
+      </c>
+      <c r="J41" s="19">
+        <f t="shared" ref="J36:J44" si="3">I41/G41</f>
+        <v>0.54428872156963</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15">
+        <v>244504</v>
+      </c>
+      <c r="E42" s="15">
+        <v>501845</v>
+      </c>
+      <c r="F42" s="15">
+        <v>267181</v>
+      </c>
+      <c r="G42" s="15">
+        <f>D42+E42-F42</f>
+        <v>479168</v>
+      </c>
+      <c r="H42" s="15">
+        <v>551355</v>
+      </c>
+      <c r="I42" s="15">
+        <f t="shared" si="2"/>
+        <v>-72187</v>
+      </c>
+      <c r="J42" s="19">
+        <f t="shared" si="3"/>
+        <v>-0.150650711232804</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15">
+        <v>267181</v>
+      </c>
+      <c r="G43" s="15">
+        <f>F43</f>
+        <v>267181</v>
+      </c>
+      <c r="H43" s="15">
+        <v>260651</v>
+      </c>
+      <c r="I43" s="15">
+        <f t="shared" si="2"/>
+        <v>6530</v>
+      </c>
+      <c r="J43" s="19">
+        <f t="shared" si="3"/>
+        <v>0.0244403606543879</v>
+      </c>
+    </row>
+    <row r="44" ht="13" customHeight="1" spans="1:10">
+      <c r="A44" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="15">
+        <f>SUM(G41:G43)</f>
+        <v>1309743</v>
+      </c>
+      <c r="H44" s="15">
+        <f>SUM(H41:H43)</f>
+        <v>1068751</v>
+      </c>
+      <c r="I44" s="15">
+        <f t="shared" si="2"/>
+        <v>240992</v>
+      </c>
+      <c r="J44" s="19">
+        <f t="shared" si="3"/>
+        <v>0.183999456381901</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="9">
+        <v>45839</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="13"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="11"/>
+      <c r="B46" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="13"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="11"/>
+      <c r="B47" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="15">
+        <v>4138375</v>
+      </c>
+      <c r="C48" s="15">
+        <v>3385980</v>
+      </c>
+      <c r="D48" s="15">
+        <v>219320</v>
+      </c>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15">
+        <f>B48-C48-D48</f>
+        <v>533075</v>
+      </c>
+      <c r="H48" s="15">
+        <v>221076</v>
+      </c>
+      <c r="I48" s="15">
+        <f t="shared" ref="I48:I51" si="4">G48-H48</f>
+        <v>311999</v>
+      </c>
+      <c r="J48" s="19">
+        <f t="shared" ref="J48:J51" si="5">I48/G48</f>
+        <v>0.585281620785068</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15">
+        <v>219320</v>
+      </c>
+      <c r="E49" s="15">
+        <v>512255</v>
+      </c>
+      <c r="F49" s="15">
+        <v>262669</v>
+      </c>
+      <c r="G49" s="15">
+        <f>D49+E49-F49</f>
+        <v>468906</v>
+      </c>
+      <c r="H49" s="15">
+        <v>516192</v>
+      </c>
+      <c r="I49" s="15">
+        <f t="shared" si="4"/>
+        <v>-47286</v>
+      </c>
+      <c r="J49" s="19">
+        <f t="shared" si="5"/>
+        <v>-0.100843239369938</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15">
+        <v>262669</v>
+      </c>
+      <c r="G50" s="15">
+        <f>F50</f>
+        <v>262669</v>
+      </c>
+      <c r="H50" s="15">
+        <v>252478</v>
+      </c>
+      <c r="I50" s="15">
+        <f t="shared" si="4"/>
+        <v>10191</v>
+      </c>
+      <c r="J50" s="19">
+        <f t="shared" si="5"/>
+        <v>0.0387978786990471</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="15">
+        <f>SUM(G48:G50)</f>
+        <v>1264650</v>
+      </c>
+      <c r="H51" s="15">
+        <f>SUM(H48:H50)</f>
+        <v>989746</v>
+      </c>
+      <c r="I51" s="15">
+        <f t="shared" si="4"/>
+        <v>274904</v>
+      </c>
+      <c r="J51" s="19">
+        <f t="shared" si="5"/>
+        <v>0.217375558454908</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="9">
+        <v>45870</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="13"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="11"/>
+      <c r="B53" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="13"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="11"/>
+      <c r="B54" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="18">
+        <v>4527304</v>
+      </c>
+      <c r="C55" s="15">
+        <v>3755221</v>
+      </c>
+      <c r="D55" s="15">
+        <v>223735</v>
+      </c>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15">
+        <f>B55-C55-D55</f>
+        <v>548348</v>
+      </c>
+      <c r="H55" s="15">
+        <v>203058</v>
+      </c>
+      <c r="I55" s="15">
+        <f t="shared" ref="I55:I58" si="6">G55-H55</f>
+        <v>345290</v>
+      </c>
+      <c r="J55" s="19">
+        <f t="shared" ref="J55:J58" si="7">I55/G55</f>
+        <v>0.629691363878413</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15">
+        <v>223735</v>
+      </c>
+      <c r="E56" s="15">
+        <v>577398</v>
+      </c>
+      <c r="F56" s="15">
+        <v>314436</v>
+      </c>
+      <c r="G56" s="15">
+        <f>D56+E56-F56</f>
+        <v>486697</v>
+      </c>
+      <c r="H56" s="15">
+        <v>507888</v>
+      </c>
+      <c r="I56" s="15">
+        <f t="shared" si="6"/>
+        <v>-21191</v>
+      </c>
+      <c r="J56" s="19">
+        <f t="shared" si="7"/>
+        <v>-0.0435404368631818</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15">
+        <v>314436</v>
+      </c>
+      <c r="G57" s="15">
+        <f>F57</f>
+        <v>314436</v>
+      </c>
+      <c r="H57" s="15">
+        <v>292381</v>
+      </c>
+      <c r="I57" s="15">
+        <f t="shared" si="6"/>
+        <v>22055</v>
+      </c>
+      <c r="J57" s="19">
+        <f t="shared" si="7"/>
+        <v>0.0701414596293045</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="15">
+        <f>SUM(G55:G57)</f>
+        <v>1349481</v>
+      </c>
+      <c r="H58" s="15">
+        <f>SUM(H55:H57)</f>
+        <v>1003327</v>
+      </c>
+      <c r="I58" s="15">
+        <f t="shared" si="6"/>
+        <v>346154</v>
+      </c>
+      <c r="J58" s="19">
+        <f t="shared" si="7"/>
+        <v>0.256508983824152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="9">
+        <v>45901</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="13"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="11"/>
+      <c r="B60" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="13"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="11"/>
+      <c r="B61" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="18">
+        <v>4264205</v>
+      </c>
+      <c r="C62" s="15">
+        <v>3457264</v>
+      </c>
+      <c r="D62" s="15">
+        <v>253250</v>
+      </c>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15">
+        <f>B62-C62-D62</f>
+        <v>553691</v>
+      </c>
+      <c r="H62" s="15">
+        <v>223896</v>
+      </c>
+      <c r="I62" s="15">
+        <f t="shared" ref="I62:I65" si="8">G62-H62</f>
+        <v>329795</v>
+      </c>
+      <c r="J62" s="19">
+        <f t="shared" ref="J62:J65" si="9">I62/G62</f>
+        <v>0.595630053585845</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15">
+        <v>253250</v>
+      </c>
+      <c r="E63" s="15">
+        <v>505577</v>
+      </c>
+      <c r="F63" s="15">
+        <v>265859</v>
+      </c>
+      <c r="G63" s="15">
+        <f>D63+E63-F63</f>
+        <v>492968</v>
+      </c>
+      <c r="H63" s="15">
+        <v>550454</v>
+      </c>
+      <c r="I63" s="15">
+        <f t="shared" si="8"/>
+        <v>-57486</v>
+      </c>
+      <c r="J63" s="19">
+        <f t="shared" si="9"/>
+        <v>-0.1166120316126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15">
+        <v>265859</v>
+      </c>
+      <c r="G64" s="15">
+        <f>F64</f>
+        <v>265859</v>
+      </c>
+      <c r="H64" s="15">
+        <v>256399</v>
+      </c>
+      <c r="I64" s="15">
+        <f t="shared" si="8"/>
+        <v>9460</v>
+      </c>
+      <c r="J64" s="19">
+        <f t="shared" si="9"/>
+        <v>0.0355827713186313</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="11"/>
+      <c r="B65" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="15">
+        <f>SUM(G62:G64)</f>
+        <v>1312518</v>
+      </c>
+      <c r="H65" s="15">
+        <f>SUM(H62:H64)</f>
+        <v>1030749</v>
+      </c>
+      <c r="I65" s="15">
+        <f t="shared" si="8"/>
+        <v>281769</v>
+      </c>
+      <c r="J65" s="19">
+        <f t="shared" si="9"/>
+        <v>0.214678198698989</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="38">
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="A9:J9"/>
     <mergeCell ref="B10:F10"/>
@@ -2166,6 +2679,23 @@
     <mergeCell ref="A31:J31"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="G32:J32"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="G46:J46"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A52:J52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A59:J59"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="G60:J60"/>
+    <mergeCell ref="B65:F65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>